<commit_message>
excel retrieving date from cell fix
</commit_message>
<xml_diff>
--- a/WebDriverTestGit/SeleniumExcelTest.xlsx
+++ b/WebDriverTestGit/SeleniumExcelTest.xlsx
@@ -18,30 +18,66 @@
     <t>Test Case Name</t>
   </si>
   <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>TestingExcel</t>
+  </si>
+  <si>
+    <t>testuser_1</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>testuser_2</t>
+  </si>
+  <si>
+    <t>testuser_3</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>leaveAComment</t>
+  </si>
+  <si>
+    <t>Bark yes for no, you nasty man</t>
+  </si>
+  <si>
+    <t>Aaron Klassen</t>
+  </si>
+  <si>
+    <t>no@email.com</t>
+  </si>
+  <si>
+    <t>http://www.google.ca</t>
+  </si>
+  <si>
+    <t>Second comment, automated response</t>
+  </si>
+  <si>
+    <t>nobody</t>
+  </si>
+  <si>
+    <t>http://www.facebook.com</t>
+  </si>
+  <si>
     <t>TestCaseName</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>TestingExcel</t>
-  </si>
-  <si>
-    <t>testuser_1</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
-  <si>
-    <t>testuser_2</t>
-  </si>
-  <si>
-    <t>testuser_3</t>
-  </si>
-  <si>
     <t>givenname</t>
   </si>
   <si>
@@ -51,12 +87,6 @@
     <t>dob</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
@@ -114,9 +144,6 @@
     <t>visa</t>
   </si>
   <si>
-    <t>Aaron Klassen</t>
-  </si>
-  <si>
     <t>0000 1234 5678 9000 0000</t>
   </si>
   <si>
@@ -129,9 +156,6 @@
     <t>anotheremail@noemail.com</t>
   </si>
   <si>
-    <t>http://www.google.ca</t>
-  </si>
-  <si>
     <t>555-4679</t>
   </si>
   <si>
@@ -142,39 +166,12 @@
   </si>
   <si>
     <t>0000 9876 5432 1000 0000</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>leaveAComment</t>
-  </si>
-  <si>
-    <t>Bark yes for no, you nasty man</t>
-  </si>
-  <si>
-    <t>no@email.com</t>
-  </si>
-  <si>
-    <t>Second comment, automated response</t>
-  </si>
-  <si>
-    <t>nobody</t>
-  </si>
-  <si>
-    <t>http://www.facebook.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-  </numFmts>
   <fonts count="10">
     <font>
       <sz val="10.0"/>
@@ -196,13 +193,6 @@
     </font>
     <font>
       <b/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <b/>
       <name val="Arial"/>
     </font>
     <font>
@@ -213,13 +203,26 @@
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <b/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -255,9 +258,6 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -268,6 +268,9 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -302,43 +305,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -364,54 +367,54 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>38</v>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>50</v>
+        <v>15</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -437,94 +440,94 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>22</v>
+      <c r="G1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="7">
-        <v>33713.0</v>
+        <v>35</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1941992.0</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H2" s="5">
         <v>10.0</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="O2" s="5">
         <v>125.0</v>
@@ -532,46 +535,46 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="7">
-        <v>34875.0</v>
+        <v>45</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1062009.0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H3" s="5">
         <v>8.0</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="K3" s="5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="O3" s="5">
         <v>824.0</v>

</xml_diff>